<commit_message>
simple directory for shortening construct names
</commit_message>
<xml_diff>
--- a/data/participant_grids/continuous/P15_clean.xlsx
+++ b/data/participant_grids/continuous/P15_clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huada\Desktop\MIT\Magic Viz\RepGridData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amyraefox/Code/MAG-Magic_Visualization/2_RepGrid_Attitudes/MAG_D/data/participant_grids/continuous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3979E299-23A0-4DA8-B6B9-80C9F2F7E219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619633D1-0351-D746-8802-7A215A82B761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14472" yWindow="528" windowWidth="14160" windowHeight="8868" xr2:uid="{F17107C7-CE15-49BB-B8A8-0D3E101BA181}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{F17107C7-CE15-49BB-B8A8-0D3E101BA181}"/>
   </bookViews>
   <sheets>
     <sheet name="P15_Grid_Cleaned" sheetId="1" r:id="rId1"/>
@@ -959,12 +959,16 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="30.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1002,7 +1006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1078,7 +1082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1116,7 +1120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1154,7 +1158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1192,7 +1196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1230,7 +1234,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>

</xml_diff>